<commit_message>
[WIP] Repurpose building to enhance bonus resource
</commit_message>
<xml_diff>
--- a/文档/资源.xlsx
+++ b/文档/资源.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\Sistine_civ6mod\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AD1DC34-74E9-4550-8C5C-374C0DBD5949}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D6E2FBF-57FC-4E33-9680-0D4A6BD60E20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="149">
   <si>
     <t>RESOURCE_BANANAS</t>
   </si>
@@ -453,10 +453,6 @@
   </si>
   <si>
     <t>工坊（锤）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>石工坊（锤）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -608,12 +604,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -630,7 +632,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -639,12 +641,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -656,6 +652,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -939,7 +944,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P12" sqref="P12"/>
+      <selection pane="bottomRight" activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -955,7 +960,7 @@
     <col min="11" max="11" width="46.21875" hidden="1" customWidth="1"/>
     <col min="12" max="13" width="9" hidden="1" customWidth="1"/>
     <col min="14" max="14" width="17.88671875" customWidth="1"/>
-    <col min="15" max="15" width="17.88671875" style="6" customWidth="1"/>
+    <col min="15" max="15" width="17.88671875" style="4" customWidth="1"/>
     <col min="16" max="16" width="12.77734375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -984,8 +989,8 @@
       <c r="N1" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="O1" s="5" t="s">
-        <v>125</v>
+      <c r="O1" s="3" t="s">
+        <v>124</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>113</v>
@@ -1008,19 +1013,19 @@
         <v>69</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="O2" s="6">
+        <v>142</v>
+      </c>
+      <c r="O2" s="4">
         <v>0</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="P2" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="Q2" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="R2" s="3" t="s">
-        <v>121</v>
+      <c r="R2" s="7" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
@@ -1049,16 +1054,16 @@
         <v>101</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="O3" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="P3" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="O3" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="P3" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="Q3" s="4"/>
-      <c r="R3" s="4"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1083,16 +1088,16 @@
         <v>101</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="O4" s="6">
+        <v>142</v>
+      </c>
+      <c r="O4" s="4">
         <v>0</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="P4" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="Q4" s="4"/>
-      <c r="R4" s="4"/>
+      <c r="Q4" s="8"/>
+      <c r="R4" s="8"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1111,16 +1116,16 @@
         <v>69</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="O5" s="6">
+        <v>142</v>
+      </c>
+      <c r="O5" s="4">
         <v>0</v>
       </c>
-      <c r="P5" s="1" t="s">
+      <c r="P5" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="Q5" s="4"/>
-      <c r="R5" s="4"/>
+      <c r="Q5" s="8"/>
+      <c r="R5" s="8"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -1139,16 +1144,16 @@
         <v>69</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="O6" s="6">
+        <v>142</v>
+      </c>
+      <c r="O6" s="4">
         <v>0</v>
       </c>
-      <c r="P6" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q6" s="4"/>
-      <c r="R6" s="4"/>
+      <c r="P6" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q6" s="8"/>
+      <c r="R6" s="8"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -1176,16 +1181,16 @@
         <v>82</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="O7" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="P7" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="O7" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="P7" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="Q7" s="4"/>
-      <c r="R7" s="4"/>
+      <c r="Q7" s="8"/>
+      <c r="R7" s="8"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -1213,16 +1218,16 @@
         <v>101</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="O8" s="6">
+        <v>142</v>
+      </c>
+      <c r="O8" s="4">
         <v>0</v>
       </c>
-      <c r="P8" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q8" s="4"/>
-      <c r="R8" s="4"/>
+      <c r="P8" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q8" s="8"/>
+      <c r="R8" s="8"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -1241,16 +1246,16 @@
         <v>101</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="O9" s="6">
+        <v>142</v>
+      </c>
+      <c r="O9" s="4">
         <v>0</v>
       </c>
-      <c r="P9" s="1" t="s">
+      <c r="P9" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="Q9" s="4"/>
-      <c r="R9" s="4"/>
+      <c r="Q9" s="8"/>
+      <c r="R9" s="8"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -1269,18 +1274,18 @@
         <v>101</v>
       </c>
       <c r="N10" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="O10" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="P10" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q10" s="8"/>
+      <c r="R10" s="8"/>
+      <c r="S10" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="O10" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="Q10" s="4"/>
-      <c r="R10" s="4"/>
-      <c r="S10" s="1" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
@@ -1300,16 +1305,16 @@
         <v>82</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="O11" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="P11" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="Q11" s="4"/>
-      <c r="R11" s="4"/>
+        <v>142</v>
+      </c>
+      <c r="O11" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="P11" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q11" s="8"/>
+      <c r="R11" s="8"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -1337,16 +1342,16 @@
         <v>101</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="O12" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="P12" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="O12" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="P12" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="Q12" s="4"/>
-      <c r="R12" s="4"/>
+      <c r="Q12" s="8"/>
+      <c r="R12" s="8"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -1359,14 +1364,14 @@
         <v>62</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="O13" s="8" t="s">
-        <v>128</v>
+        <v>142</v>
+      </c>
+      <c r="O13" s="6" t="s">
+        <v>127</v>
       </c>
       <c r="P13" s="1"/>
-      <c r="Q13" s="3" t="s">
-        <v>124</v>
+      <c r="Q13" s="7" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
@@ -1382,10 +1387,10 @@
       <c r="N14" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="O14" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="Q14" s="4"/>
+      <c r="O14" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="Q14" s="8"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -1398,12 +1403,12 @@
         <v>108</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="O15" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="Q15" s="4"/>
+        <v>146</v>
+      </c>
+      <c r="O15" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q15" s="8"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -1418,10 +1423,10 @@
       <c r="N16" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="O16" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="Q16" s="4"/>
+      <c r="O16" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q16" s="8"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -1454,10 +1459,10 @@
       <c r="N17" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="O17" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="Q17" s="4"/>
+      <c r="O17" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q17" s="8"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -1479,12 +1484,12 @@
         <v>109</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="O18" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q18" s="4"/>
+        <v>145</v>
+      </c>
+      <c r="O18" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q18" s="8"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -1509,12 +1514,12 @@
         <v>86</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="O19" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q19" s="4"/>
+        <v>144</v>
+      </c>
+      <c r="O19" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q19" s="8"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -1529,10 +1534,10 @@
       <c r="N20" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="O20" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="Q20" s="4"/>
+      <c r="O20" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q20" s="8"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
@@ -1554,12 +1559,12 @@
         <v>109</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="O21" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="Q21" s="4"/>
+        <v>147</v>
+      </c>
+      <c r="O21" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q21" s="8"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -1580,10 +1585,10 @@
       <c r="N22" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="O22" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="Q22" s="4"/>
+      <c r="O22" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q22" s="8"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
@@ -1596,12 +1601,12 @@
         <v>108</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="O23" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="Q23" s="4"/>
+        <v>146</v>
+      </c>
+      <c r="O23" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q23" s="8"/>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
@@ -1620,12 +1625,12 @@
         <v>108</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="O24" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="Q24" s="4"/>
+        <v>146</v>
+      </c>
+      <c r="O24" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q24" s="8"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -1638,12 +1643,12 @@
         <v>110</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="O25" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="Q25" s="4"/>
+        <v>148</v>
+      </c>
+      <c r="O25" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q25" s="8"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
@@ -1662,12 +1667,12 @@
         <v>109</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="O26" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="Q26" s="4"/>
+        <v>145</v>
+      </c>
+      <c r="O26" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q26" s="8"/>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
@@ -1682,10 +1687,10 @@
       <c r="N27" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="O27" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="Q27" s="4"/>
+      <c r="O27" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q27" s="8"/>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
@@ -1710,12 +1715,12 @@
         <v>108</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="O28" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="Q28" s="4"/>
+        <v>146</v>
+      </c>
+      <c r="O28" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q28" s="8"/>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
@@ -1736,10 +1741,10 @@
       <c r="N29" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="O29" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="Q29" s="4"/>
+      <c r="O29" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q29" s="8"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
@@ -1764,12 +1769,12 @@
         <v>62</v>
       </c>
       <c r="N30" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="O30" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q30" s="4"/>
+        <v>142</v>
+      </c>
+      <c r="O30" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q30" s="8"/>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
@@ -1791,12 +1796,12 @@
         <v>62</v>
       </c>
       <c r="N31" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="O31" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="Q31" s="4"/>
+        <v>142</v>
+      </c>
+      <c r="O31" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q31" s="8"/>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
@@ -1809,12 +1814,12 @@
         <v>110</v>
       </c>
       <c r="N32" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="O32" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="Q32" s="4"/>
+        <v>148</v>
+      </c>
+      <c r="O32" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q32" s="8"/>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
@@ -1830,12 +1835,12 @@
         <v>109</v>
       </c>
       <c r="N33" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="O33" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="Q33" s="4"/>
+        <v>145</v>
+      </c>
+      <c r="O33" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q33" s="8"/>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
@@ -1850,10 +1855,10 @@
       <c r="N34" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="O34" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="Q34" s="4"/>
+      <c r="O34" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q34" s="8"/>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
@@ -1881,10 +1886,10 @@
       <c r="N35" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="O35" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="Q35" s="4"/>
+      <c r="O35" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q35" s="8"/>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
@@ -1909,12 +1914,12 @@
         <v>86</v>
       </c>
       <c r="N36" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="O36" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="Q36" s="4"/>
+        <v>144</v>
+      </c>
+      <c r="O36" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q36" s="8"/>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
@@ -1927,12 +1932,12 @@
         <v>108</v>
       </c>
       <c r="N37" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="O37" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="Q37" s="4"/>
+        <v>146</v>
+      </c>
+      <c r="O37" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q37" s="8"/>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
@@ -1947,10 +1952,10 @@
       <c r="N38" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="O38" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="Q38" s="4"/>
+      <c r="O38" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q38" s="8"/>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
@@ -1963,12 +1968,12 @@
         <v>110</v>
       </c>
       <c r="N39" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="O39" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="Q39" s="4"/>
+        <v>148</v>
+      </c>
+      <c r="O39" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="Q39" s="8"/>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
@@ -1981,12 +1986,12 @@
         <v>62</v>
       </c>
       <c r="N40" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="O40" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="Q40" s="4"/>
+        <v>142</v>
+      </c>
+      <c r="O40" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q40" s="8"/>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
@@ -2008,11 +2013,11 @@
         <v>110</v>
       </c>
       <c r="N41" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="O41" s="6"/>
+      <c r="Q41" s="7" t="s">
         <v>122</v>
-      </c>
-      <c r="O41" s="8"/>
-      <c r="Q41" s="3" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.25">
@@ -2041,10 +2046,10 @@
         <v>61</v>
       </c>
       <c r="N42" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="O42" s="8"/>
-      <c r="Q42" s="4"/>
+        <v>142</v>
+      </c>
+      <c r="O42" s="6"/>
+      <c r="Q42" s="8"/>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
@@ -2071,8 +2076,8 @@
       <c r="N43" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="O43" s="8"/>
-      <c r="Q43" s="4"/>
+      <c r="O43" s="6"/>
+      <c r="Q43" s="8"/>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
@@ -2097,10 +2102,10 @@
         <v>110</v>
       </c>
       <c r="N44" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="O44" s="8"/>
-      <c r="Q44" s="4"/>
+        <v>121</v>
+      </c>
+      <c r="O44" s="6"/>
+      <c r="Q44" s="8"/>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
@@ -2118,8 +2123,8 @@
       <c r="N45" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="O45" s="8"/>
-      <c r="Q45" s="4"/>
+      <c r="O45" s="6"/>
+      <c r="Q45" s="8"/>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
@@ -2147,10 +2152,10 @@
         <v>73</v>
       </c>
       <c r="N46" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="O46" s="8"/>
-      <c r="Q46" s="4"/>
+        <v>142</v>
+      </c>
+      <c r="O46" s="6"/>
+      <c r="Q46" s="8"/>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
@@ -2172,10 +2177,10 @@
         <v>61</v>
       </c>
       <c r="N47" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="O47" s="8"/>
-      <c r="Q47" s="4"/>
+        <v>142</v>
+      </c>
+      <c r="O47" s="6"/>
+      <c r="Q47" s="8"/>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">

</xml_diff>